<commit_message>
Uploading solutions Functions and Statements Lab
</commit_message>
<xml_diff>
--- a/JavaScript.xlsx
+++ b/JavaScript.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>ShortCuts</t>
   </si>
@@ -259,6 +259,38 @@
   </si>
   <si>
     <t>Връща масива филтриран по даден елемент, в случая ако в него има "undefined"</t>
+  </si>
+  <si>
+    <t>function calculaton(num1, num2, opr){
+    let result = {
+        'multiply': (a, b) =&gt; a * b,
+        'divide': (a, b) =&gt; a / b,
+        'add': (a, b) =&gt; a + b,
+        'subtract': (a, b) =&gt; a - b
+    }
+    console.log(result[opr](num1, num2));
+}</t>
+  </si>
+  <si>
+    <t>Калкоратор чрез речник без if - else проверки с използването на arow function</t>
+  </si>
+  <si>
+    <t>chr1.charCodeAt(0);</t>
+  </si>
+  <si>
+    <t>Връща ASCII стойността на символа.</t>
+  </si>
+  <si>
+    <t>String.fromCharCode(i);</t>
+  </si>
+  <si>
+    <t>Връща символ от ASCII таблицата по зададено число.</t>
+  </si>
+  <si>
+    <t>let numArr = String(num).split("").map((num) =&gt; Number(num))</t>
+  </si>
+  <si>
+    <t>Превръща число в масив от числа . 12345 - [1, 2, 3, 4, 5]</t>
   </si>
 </sst>
 </file>
@@ -323,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -346,6 +378,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -627,15 +662,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B43"/>
+  <dimension ref="A2:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="58.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="70.109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="97.5546875" style="4" customWidth="1"/>
     <col min="3" max="16384" width="8.88671875" style="3"/>
   </cols>
@@ -842,87 +877,119 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
+    <row r="31" spans="1:2" ht="148.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="6"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B32" s="6"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>52</v>
+        <v>42</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A41" s="7" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A43" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="8"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+      <c r="B43" s="8"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A32:B32"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A43:B43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Uploading Objects and Classes - Lab
</commit_message>
<xml_diff>
--- a/JavaScript.xlsx
+++ b/JavaScript.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="113">
   <si>
     <t>ShortCuts</t>
   </si>
@@ -270,9 +270,6 @@
     }
     console.log(result[opr](num1, num2));
 }</t>
-  </si>
-  <si>
-    <t>Калкоратор чрез речник без if - else проверки с използването на arow function</t>
   </si>
   <si>
     <t>chr1.charCodeAt(0);</t>
@@ -340,12 +337,184 @@
   <si>
     <t>Ревърсва думата</t>
   </si>
+  <si>
+    <t>Objects</t>
+  </si>
+  <si>
+    <t>Object.keys(dict);</t>
+  </si>
+  <si>
+    <t>връща ключовете на речника</t>
+  </si>
+  <si>
+    <t>Object.values(dict);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">връща стойностите </t>
+  </si>
+  <si>
+    <t>Object.entries(dict);</t>
+  </si>
+  <si>
+    <t>връща списък от списъци с ключ и стойност [[key1, value1], [key2, value2]]. Python - dict.items() - връща списък от тюпъли.</t>
+  </si>
+  <si>
+    <t>for(const [index, name] of names.entries())</t>
+  </si>
+  <si>
+    <t>Python - enumerate</t>
+  </si>
+  <si>
+    <t>#word.slice(1); -- wod</t>
+  </si>
+  <si>
+    <t>връща думата без първия символ</t>
+  </si>
+  <si>
+    <t>function cityInfo(data){
+    for (const [key, value] of Object.entries(data)) {
+        console.log(`${key} -&gt; ${value}`);   
+    }
+};</t>
+  </si>
+  <si>
+    <t>Итериране през обект, взимаме ключа и стойноста</t>
+  </si>
+  <si>
+    <r>
+      <t>function cityInfo(data){
+    for (const key of Object.keys(data)) {
+        console.log(`${key} -&gt; ${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>data[key]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">}`);   
+    }
+}; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>data.key</t>
+    </r>
+  </si>
+  <si>
+    <t>Два начина за достъпване на стойност. data.key , data[key]</t>
+  </si>
+  <si>
+    <t>let person = {
+       firstName: firstName,
+        lastName: lastName,
+        age: age,
+    };</t>
+  </si>
+  <si>
+    <t>let dict = { name, surName, age}</t>
+  </si>
+  <si>
+    <t>Ако имената на ключовете и стойностите съвпадат може да се напише и така. Това съсдава обект с ключ name и стойност name</t>
+  </si>
+  <si>
+    <t>Калкулатор чрез речник без if - else проверки с използването на arow function</t>
+  </si>
+  <si>
+    <t>let cityInfo = {
+        "name": name,
+        "population": population,
+        "treasury": treasury,
+        "taxRate": 10,
+        collectTaxes(){
+            this.treasury += this.population * this.taxRate
+        },
+        applyGrowth(percentage){
+            percentage /= 100;
+            this.population *= percentage + 1;
+        },
+        applyRecession(percentage){
+            percentage /= 100;
+           this.treasury *= 1 - percentage;
+        }
+    };</t>
+  </si>
+  <si>
+    <t>Методи на обект</t>
+  </si>
+  <si>
+    <t>let person = JSON.parse(jsonStr);</t>
+  </si>
+  <si>
+    <t>Конвертира json string в обект (речник)</t>
+  </si>
+  <si>
+    <t>person.sayHello = () =&gt; console.log("Hello");</t>
+  </si>
+  <si>
+    <t>Добавяне на метод към съществуващ обект.</t>
+  </si>
+  <si>
+    <t>let person = { firstName, lastName, age};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Създава речник Когато ключовете и стойностите са с еднакви имена на променливите. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> const sortedAddressBook = Object.keys(addressBook).sort().reduce(
+        (obj, key) =&gt; { 
+          obj[key] = addressBook[key]; 
+          return obj;
+        }, 
+        {}
+      );</t>
+  </si>
+  <si>
+    <t>Сортиране на обект по ключ по азбучен ред</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>class Cat{
+        constructor(name, age){
+            this.name = name;
+            this.age = age;
+        }</t>
+  </si>
+  <si>
+    <t>Създаване на клас</t>
+  </si>
+  <si>
+    <t>songs.forEach((song) =&gt; console.log(song.name));</t>
+  </si>
+  <si>
+    <t>Принтиране на елементи от масив с обекти чрез  foreach</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,6 +559,13 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -411,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -437,6 +613,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -718,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B47"/>
+  <dimension ref="A2:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -935,146 +1117,286 @@
     </row>
     <row r="29" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+    </row>
+    <row r="31" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="148.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+    <row r="32" spans="1:2" ht="148.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
+      <c r="B32" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="7"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="B33" s="7"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>10</v>
+        <v>46</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>51</v>
+        <v>42</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>52</v>
+        <v>88</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="78" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
         <v>77</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="78" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="4" t="s">
+    </row>
+    <row r="45" spans="1:2" ht="61.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="9"/>
+    </row>
+    <row r="46" spans="1:2" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" s="11"/>
+    </row>
+    <row r="47" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="78" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="78" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="265.2" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A60" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B60" s="9"/>
+    </row>
+    <row r="61" spans="1:2" ht="78" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A64" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B64" s="9"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B67" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A44" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B44" s="9"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A32:B32"/>
+  <mergeCells count="5">
+    <mergeCell ref="A33:B33"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A60:B60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add solutions from the Exercise
</commit_message>
<xml_diff>
--- a/JavaScript.xlsx
+++ b/JavaScript.xlsx
@@ -602,6 +602,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -613,12 +619,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -982,10 +982,10 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="22.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="11"/>
     </row>
     <row r="13" spans="1:2" ht="82.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -1148,10 +1148,10 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="7"/>
+      <c r="B33" s="9"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
@@ -1165,7 +1165,7 @@
       <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1173,7 +1173,7 @@
       <c r="A36" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="6" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1181,7 +1181,7 @@
       <c r="A37" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="6" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1239,30 +1239,30 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="61.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="9"/>
+      <c r="B45" s="11"/>
     </row>
     <row r="46" spans="1:2" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="11"/>
+      <c r="B46" s="7"/>
     </row>
     <row r="47" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="7" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="6" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1339,10 +1339,10 @@
       </c>
     </row>
     <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A60" s="8" t="s">
+      <c r="A60" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B60" s="9"/>
+      <c r="B60" s="11"/>
     </row>
     <row r="61" spans="1:2" ht="78" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
@@ -1361,10 +1361,10 @@
       </c>
     </row>
     <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A64" s="8" t="s">
+      <c r="A64" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B64" s="9"/>
+      <c r="B64" s="11"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">

</xml_diff>

<commit_message>
add solutions of DOM Events
</commit_message>
<xml_diff>
--- a/JavaScript.xlsx
+++ b/JavaScript.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3E3E88-9EB3-477A-8281-E9438F283B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F77C9D0-8511-4AF7-9E6B-3A11D6D0D582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="465" windowWidth="21630" windowHeight="16935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="149">
   <si>
     <t>ShortCuts</t>
   </si>
@@ -634,6 +634,9 @@
   </si>
   <si>
     <t>Добавяне на клас на перант елемент при фокусиране на child елемент</t>
+  </si>
+  <si>
+    <t>let email = document.getElementsByName("email")[0].value;</t>
   </si>
 </sst>
 </file>
@@ -1038,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B86"/>
+  <dimension ref="A2:B87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1675,6 +1678,14 @@
         <v>144</v>
       </c>
       <c r="B86" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B87" s="4" t="s">
         <v>145</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update solution 04. Post
</commit_message>
<xml_diff>
--- a/JavaScript.xlsx
+++ b/JavaScript.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E13614-12FB-44BA-9F58-72E299578BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="186">
   <si>
     <t>ShortCuts</t>
   </si>
@@ -789,11 +790,20 @@
   <si>
     <t>селектира елемента с име имейл.</t>
   </si>
+  <si>
+    <t>h1.textContent = document.querySelector(`#posts option[value=${postId}`).textContent;</t>
+  </si>
+  <si>
+    <t>Взимане на сойност чрез иинтерполация с променлива</t>
+  </si>
+  <si>
+    <t>h1.textContent =  optionElement.selectedOptions[0].textContent;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -929,6 +939,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -936,9 +949,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1223,27 +1233,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B113"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:B115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="95.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="97.5546875" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="95.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="97.5703125" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1251,7 +1261,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1259,7 +1269,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1267,7 +1277,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1275,7 +1285,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
@@ -1283,13 +1293,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>145</v>
       </c>
@@ -1297,7 +1307,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -1305,13 +1315,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="22.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="22.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="14"/>
-    </row>
-    <row r="13" spans="1:2" ht="82.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="15"/>
+    </row>
+    <row r="13" spans="1:2" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>32</v>
       </c>
@@ -1319,7 +1329,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>133</v>
       </c>
@@ -1327,7 +1337,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>139</v>
       </c>
@@ -1335,7 +1345,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>143</v>
       </c>
@@ -1343,7 +1353,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>131</v>
       </c>
@@ -1351,7 +1361,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>135</v>
       </c>
@@ -1359,7 +1369,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>141</v>
       </c>
@@ -1367,7 +1377,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
@@ -1375,17 +1385,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13" t="s">
+    <row r="21" spans="1:2" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="B21" s="14"/>
-    </row>
-    <row r="22" spans="1:2" s="9" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="15"/>
+    </row>
+    <row r="22" spans="1:2" s="9" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="12"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>160</v>
       </c>
@@ -1393,10 +1403,10 @@
         <v>159</v>
       </c>
     </row>
-    <row r="24" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="1:2" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>161</v>
       </c>
@@ -1404,10 +1414,10 @@
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
     </row>
-    <row r="27" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>163</v>
       </c>
@@ -1415,10 +1425,10 @@
         <v>164</v>
       </c>
     </row>
-    <row r="28" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>165</v>
       </c>
@@ -1426,10 +1436,10 @@
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>167</v>
       </c>
@@ -1437,10 +1447,10 @@
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>169</v>
       </c>
@@ -1448,10 +1458,10 @@
         <v>170</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>138</v>
       </c>
@@ -1459,7 +1469,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>137</v>
       </c>
@@ -1467,7 +1477,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>34</v>
       </c>
@@ -1475,7 +1485,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>15</v>
       </c>
@@ -1483,7 +1493,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>17</v>
       </c>
@@ -1491,7 +1501,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>19</v>
       </c>
@@ -1499,7 +1509,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>27</v>
       </c>
@@ -1507,7 +1517,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>29</v>
       </c>
@@ -1515,7 +1525,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>25</v>
       </c>
@@ -1523,7 +1533,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>21</v>
       </c>
@@ -1531,7 +1541,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>23</v>
       </c>
@@ -1539,7 +1549,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>37</v>
       </c>
@@ -1547,7 +1557,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>156</v>
       </c>
@@ -1555,7 +1565,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>38</v>
       </c>
@@ -1563,7 +1573,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>42</v>
       </c>
@@ -1571,7 +1581,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>61</v>
       </c>
@@ -1579,7 +1589,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>84</v>
       </c>
@@ -1587,7 +1597,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>68</v>
       </c>
@@ -1595,7 +1605,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>152</v>
       </c>
@@ -1603,7 +1613,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>59</v>
       </c>
@@ -1611,7 +1621,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="148.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" ht="148.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>63</v>
       </c>
@@ -1619,7 +1629,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="148.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" ht="148.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>115</v>
       </c>
@@ -1627,7 +1637,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>119</v>
       </c>
@@ -1635,13 +1645,13 @@
         <v>120</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="15" t="s">
+    <row r="62" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B62" s="16"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B62" s="13"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>44</v>
       </c>
@@ -1649,7 +1659,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>40</v>
       </c>
@@ -1657,7 +1667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>86</v>
       </c>
@@ -1665,7 +1675,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>48</v>
       </c>
@@ -1673,7 +1683,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>51</v>
       </c>
@@ -1681,7 +1691,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>52</v>
       </c>
@@ -1689,7 +1699,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>64</v>
       </c>
@@ -1697,7 +1707,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>75</v>
       </c>
@@ -1705,7 +1715,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>66</v>
       </c>
@@ -1713,12 +1723,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="91.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>122</v>
       </c>
@@ -1726,7 +1736,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>123</v>
       </c>
@@ -1734,7 +1744,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>124</v>
       </c>
@@ -1742,7 +1752,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>128</v>
       </c>
@@ -1750,7 +1760,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>68</v>
       </c>
@@ -1758,7 +1768,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>70</v>
       </c>
@@ -1766,19 +1776,19 @@
         <v>71</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="61.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" ht="61.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B79" s="14"/>
-    </row>
-    <row r="80" spans="1:2" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="15"/>
+    </row>
+    <row r="80" spans="1:2" ht="61.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>92</v>
       </c>
       <c r="B80" s="7"/>
     </row>
-    <row r="81" spans="1:2" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>102</v>
       </c>
@@ -1786,7 +1796,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" ht="61.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>93</v>
       </c>
@@ -1794,7 +1804,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>78</v>
       </c>
@@ -1802,7 +1812,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>80</v>
       </c>
@@ -1810,7 +1820,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>104</v>
       </c>
@@ -1818,7 +1828,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>149</v>
       </c>
@@ -1826,7 +1836,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>150</v>
       </c>
@@ -1834,7 +1844,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>154</v>
       </c>
@@ -1842,7 +1852,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="78" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>90</v>
       </c>
@@ -1850,7 +1860,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>82</v>
       </c>
@@ -1858,7 +1868,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="78" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>88</v>
       </c>
@@ -1866,7 +1876,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="265.2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>96</v>
       </c>
@@ -1874,7 +1884,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>114</v>
       </c>
@@ -1882,7 +1892,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>98</v>
       </c>
@@ -1890,7 +1900,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>100</v>
       </c>
@@ -1898,7 +1908,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>117</v>
       </c>
@@ -1906,7 +1916,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>146</v>
       </c>
@@ -1914,13 +1924,13 @@
         <v>147</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A98" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B98" s="14"/>
-    </row>
-    <row r="99" spans="1:2" ht="78" x14ac:dyDescent="0.3">
+      <c r="B98" s="15"/>
+    </row>
+    <row r="99" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>107</v>
       </c>
@@ -1928,7 +1938,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>109</v>
       </c>
@@ -1936,7 +1946,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>111</v>
       </c>
@@ -1944,13 +1954,13 @@
         <v>112</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A102" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B102" s="14"/>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B102" s="15"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>55</v>
       </c>
@@ -1958,7 +1968,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>57</v>
       </c>
@@ -1966,7 +1976,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>73</v>
       </c>
@@ -1974,7 +1984,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>129</v>
       </c>
@@ -1982,7 +1992,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>179</v>
       </c>
@@ -1990,13 +2000,13 @@
         <v>180</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="13" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="B108" s="14"/>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B108" s="15"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>171</v>
       </c>
@@ -2004,7 +2014,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>173</v>
       </c>
@@ -2012,7 +2022,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>175</v>
       </c>
@@ -2020,7 +2030,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>176</v>
       </c>
@@ -2028,7 +2038,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>181</v>
       </c>
@@ -2036,8 +2046,23 @@
         <v>182</v>
       </c>
     </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B114" s="13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B115" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="B114:B115"/>
     <mergeCell ref="A108:B108"/>
     <mergeCell ref="A62:B62"/>
     <mergeCell ref="A12:B12"/>

</xml_diff>

<commit_message>
Uploading solution 06.Phone book
</commit_message>
<xml_diff>
--- a/JavaScript.xlsx
+++ b/JavaScript.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A5514D-6B63-4DD0-BF08-27A1F56F0974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C900A6-4830-4415-AC51-A682AF8AE8B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="465" windowWidth="21630" windowHeight="16935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="195">
   <si>
     <t>ShortCuts</t>
   </si>
@@ -815,6 +815,31 @@
             body: JSON.stringify(body)
         });
         const data = await response.json();</t>
+  </si>
+  <si>
+    <t>const content = Object.values(data).map(entry =&gt; `${entry.author}: ${entry.content}`).join('\n');</t>
+  </si>
+  <si>
+    <t>Обхождане на обект с обекти и създаване на масив със съдържанието на обектите</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> const content = [];
+ for (const elem of Object.values(data)) {
+            content.push(`${elem.author}: ${elem.content}`)
+        }</t>
+  </si>
+  <si>
+    <t>let li = e.currentTarget.parentElement;
+let id = li.getAttribute('data-id');</t>
+  </si>
+  <si>
+    <t>Изтриване на елемент от сървъра .</t>
+  </si>
+  <si>
+    <t>let id = li.getAttribute('data-id');</t>
+  </si>
+  <si>
+    <t>Взимане на атрибут на елемент</t>
   </si>
 </sst>
 </file>
@@ -1251,10 +1276,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B116"/>
+  <dimension ref="A2:B120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2085,8 +2110,39 @@
         <v>186</v>
       </c>
     </row>
+    <row r="117" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B117" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B118" s="13"/>
+    </row>
+    <row r="119" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A119" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="B117:B118"/>
     <mergeCell ref="B114:B115"/>
     <mergeCell ref="A108:B108"/>
     <mergeCell ref="A62:B62"/>

</xml_diff>

<commit_message>
Upload solution Problem 3 – Grocery List
</commit_message>
<xml_diff>
--- a/JavaScript.xlsx
+++ b/JavaScript.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5922A74-CF22-46FD-A374-A0FBA737154C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E2C8E6-4A04-45D1-B300-EAF3D3200F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="465" windowWidth="21630" windowHeight="16935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="207">
   <si>
     <t>ShortCuts</t>
   </si>
@@ -893,6 +893,12 @@
         }
         return newElement;
     }</t>
+  </si>
+  <si>
+    <t>productName.value = tr.children[0].textContent;</t>
+  </si>
+  <si>
+    <t>достъпване до child емент</t>
   </si>
 </sst>
 </file>
@@ -1336,10 +1342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B127"/>
+  <dimension ref="A2:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2249,6 +2255,14 @@
     <row r="127" spans="1:2" ht="299.25" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>204</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uplading solution of CarDealer
</commit_message>
<xml_diff>
--- a/JavaScript.xlsx
+++ b/JavaScript.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6EFD9C-FDF2-4D0C-A9DD-7A6559EA5443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305F25D1-5E10-4C16-A844-F791729E80A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="465" windowWidth="21630" windowHeight="16935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1142,20 +1142,20 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1439,8 +1439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1519,10 +1519,10 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="22.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="19"/>
+      <c r="B12" s="20"/>
     </row>
     <row r="13" spans="1:2" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1589,10 +1589,10 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="B21" s="19"/>
+      <c r="B21" s="20"/>
     </row>
     <row r="22" spans="1:2" s="9" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
@@ -1849,10 +1849,10 @@
       </c>
     </row>
     <row r="62" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="22" t="s">
+      <c r="A62" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B62" s="21"/>
+      <c r="B62" s="18"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
@@ -1980,10 +1980,10 @@
       </c>
     </row>
     <row r="79" spans="1:2" ht="61.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="18" t="s">
+      <c r="A79" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B79" s="19"/>
+      <c r="B79" s="20"/>
     </row>
     <row r="80" spans="1:2" ht="61.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
@@ -2136,10 +2136,10 @@
       </c>
     </row>
     <row r="99" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A99" s="18" t="s">
+      <c r="A99" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="B99" s="19"/>
+      <c r="B99" s="20"/>
     </row>
     <row r="100" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
@@ -2166,10 +2166,10 @@
       </c>
     </row>
     <row r="103" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A103" s="18" t="s">
+      <c r="A103" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B103" s="19"/>
+      <c r="B103" s="20"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
@@ -2212,10 +2212,10 @@
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="20" t="s">
+      <c r="A109" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="B109" s="19"/>
+      <c r="B109" s="20"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
@@ -2269,7 +2269,7 @@
       <c r="A116" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B116" s="21" t="s">
+      <c r="B116" s="18" t="s">
         <v>184</v>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       <c r="A117" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B117" s="21"/>
+      <c r="B117" s="18"/>
     </row>
     <row r="118" spans="1:2" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
@@ -2291,7 +2291,7 @@
       <c r="A119" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B119" s="21" t="s">
+      <c r="B119" s="18" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2299,7 +2299,7 @@
       <c r="A120" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B120" s="21"/>
+      <c r="B120" s="18"/>
     </row>
     <row r="121" spans="1:2" ht="126" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
@@ -2313,7 +2313,7 @@
       <c r="A122" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="B122" s="21" t="s">
+      <c r="B122" s="18" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2321,7 +2321,7 @@
       <c r="A123" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="B123" s="21"/>
+      <c r="B123" s="18"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
@@ -2414,16 +2414,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A21:B21"/>
     <mergeCell ref="B122:B123"/>
     <mergeCell ref="B119:B120"/>
     <mergeCell ref="B116:B117"/>
     <mergeCell ref="A109:B109"/>
     <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A21:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>

</xml_diff>